<commit_message>
Results for alpha = 0.01 -- not very good for the joint model
</commit_message>
<xml_diff>
--- a/tuning/alpha_tuning_joint.xlsx
+++ b/tuning/alpha_tuning_joint.xlsx
@@ -497,6 +497,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>26565.7975693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24377.3680291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24560.7594295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24453.998558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24744.0533018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24549.5441608</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24553.8706493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23936.5731478</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24190.8561316</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22814.6516104</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23255.7587996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23231.3569994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23160.6402683</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24986.9566936</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22978.0805016</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23113.1382852</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23313.9190412</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22632.9259491</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23201.073472</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22742.8499775</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1671,7 +1731,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,6 +1763,9 @@
       <c r="B2">
         <v>14597.2498674</v>
       </c>
+      <c r="E2">
+        <v>26565.797569300001</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1711,6 +1774,9 @@
       <c r="B3">
         <v>11247.5414028</v>
       </c>
+      <c r="E3">
+        <v>24377.368029099998</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1719,6 +1785,9 @@
       <c r="B4">
         <v>10067.8993931</v>
       </c>
+      <c r="E4">
+        <v>24560.759429500002</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1727,6 +1796,9 @@
       <c r="B5">
         <v>9398.4562315900002</v>
       </c>
+      <c r="E5">
+        <v>24453.998557999999</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1735,6 +1807,9 @@
       <c r="B6">
         <v>8926.7605438200007</v>
       </c>
+      <c r="E6">
+        <v>24744.053301799999</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1743,6 +1818,9 @@
       <c r="B7">
         <v>8767.0897145300005</v>
       </c>
+      <c r="E7">
+        <v>24549.5441608</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1751,6 +1829,9 @@
       <c r="B8">
         <v>8485.2773580600006</v>
       </c>
+      <c r="E8">
+        <v>24553.870649299999</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1759,6 +1840,9 @@
       <c r="B9">
         <v>8349.7820348700006</v>
       </c>
+      <c r="E9">
+        <v>23936.573147800002</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1767,6 +1851,9 @@
       <c r="B10">
         <v>8263.8935527800004</v>
       </c>
+      <c r="E10">
+        <v>24190.856131600001</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1775,6 +1862,9 @@
       <c r="B11">
         <v>8190.7684907900002</v>
       </c>
+      <c r="E11">
+        <v>22814.6516104</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1783,6 +1873,9 @@
       <c r="B12">
         <v>8223.3691778199991</v>
       </c>
+      <c r="E12">
+        <v>23255.7587996</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1791,6 +1884,9 @@
       <c r="B13">
         <v>8163.5034904499998</v>
       </c>
+      <c r="E13">
+        <v>23231.356999399999</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1799,6 +1895,9 @@
       <c r="B14">
         <v>8003.7875513999998</v>
       </c>
+      <c r="E14">
+        <v>23160.640268300001</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1807,6 +1906,9 @@
       <c r="B15">
         <v>8066.2103843699997</v>
       </c>
+      <c r="E15">
+        <v>24986.956693600001</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1815,48 +1917,66 @@
       <c r="B16">
         <v>7956.8879795100002</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>22978.080501600001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>160</v>
       </c>
       <c r="B17">
         <v>7906.24143362</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>23113.138285199999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>170</v>
       </c>
       <c r="B18">
         <v>7847.0773320199996</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>23313.919041199999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>180</v>
       </c>
       <c r="B19">
         <v>7810.1063852300003</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>22632.925949100001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>190</v>
       </c>
       <c r="B20">
         <v>7705.1879444099995</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>23201.073472</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>200</v>
       </c>
       <c r="B21">
         <v>7798.8757062000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>22742.849977499998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>

</xml_diff>